<commit_message>
Troca do tipo de gráfico de dc.barChart para dc.lineChart e refatoração de várias duplicidades de código.
</commit_message>
<xml_diff>
--- a/mono/cronograma tcc Glauber Gadelha - 2015790028  - 2019-02.xlsx
+++ b/mono/cronograma tcc Glauber Gadelha - 2015790028  - 2019-02.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="125" documentId="11_D6A0EA3B4775B8CC83F522E5F45E4A6C769F18B8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F3DC405E-EF6F-43EE-AAC8-32A725BCB2C0}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -134,8 +133,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,9 +393,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -434,9 +433,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -469,26 +468,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -521,26 +503,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -713,14 +678,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="13" customWidth="1"/>
@@ -730,7 +695,7 @@
     <col min="19" max="19" width="12.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75">
+    <row r="1" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -741,7 +706,7 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:19" ht="15.75">
+    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
@@ -755,7 +720,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -788,7 +753,7 @@
       </c>
       <c r="S4" s="28"/>
     </row>
-    <row r="5" spans="1:19" ht="25.5">
+    <row r="5" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
       <c r="B5" s="7" t="s">
         <v>5</v>
@@ -845,7 +810,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
@@ -868,7 +833,7 @@
       <c r="R6" s="10"/>
       <c r="S6" s="25"/>
     </row>
-    <row r="7" spans="1:19" ht="30">
+    <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
@@ -891,7 +856,7 @@
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
@@ -914,7 +879,7 @@
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
     </row>
-    <row r="9" spans="1:19" ht="30">
+    <row r="9" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
@@ -937,7 +902,7 @@
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
     </row>
-    <row r="10" spans="1:19" ht="30">
+    <row r="10" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -960,7 +925,7 @@
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
     </row>
-    <row r="11" spans="1:19" ht="59.25" customHeight="1">
+    <row r="11" spans="1:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
@@ -983,7 +948,7 @@
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
@@ -1006,7 +971,7 @@
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>30</v>
       </c>
@@ -1029,7 +994,7 @@
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
@@ -1052,7 +1017,7 @@
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
@@ -1075,7 +1040,7 @@
       <c r="R15" s="11"/>
       <c r="S15" s="10"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
@@ -1098,7 +1063,7 @@
       <c r="R16" s="10"/>
       <c r="S16" s="11"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="17"/>
       <c r="C17" s="12"/>
@@ -1119,7 +1084,7 @@
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="17"/>
       <c r="C18" s="12"/>
@@ -1140,7 +1105,7 @@
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="17"/>
       <c r="C19" s="12"/>
@@ -1161,7 +1126,7 @@
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="17"/>
       <c r="C20" s="12"/>
@@ -1182,7 +1147,7 @@
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="17"/>
       <c r="C21" s="12"/>
@@ -1203,7 +1168,7 @@
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="17"/>
       <c r="C22" s="12"/>
@@ -1224,7 +1189,7 @@
       <c r="R22" s="12"/>
       <c r="S22" s="12"/>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="17"/>
       <c r="C23" s="12"/>
@@ -1245,7 +1210,7 @@
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="18"/>
       <c r="C24" s="12"/>
@@ -1266,7 +1231,7 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="18"/>
       <c r="C25" s="12"/>
@@ -1287,7 +1252,7 @@
       <c r="R25" s="12"/>
       <c r="S25" s="12"/>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="18"/>
       <c r="C26" s="12"/>
@@ -1323,12 +1288,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1336,12 +1301,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>